<commit_message>
use GraphQL for the fetching posts
</commit_message>
<xml_diff>
--- a/spec/spec.xlsx
+++ b/spec/spec.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shota\Desktop\travelr\spec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D3FC4F2-9971-4DF8-B7EE-73AF48C2F576}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8C07C99-F36B-49B4-B38F-A5F0AEABB2E3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25860" windowHeight="11830" activeTab="1" xr2:uid="{6B85AF98-9DCB-4943-BC09-B1016EC709F7}"/>
   </bookViews>
@@ -3958,18 +3958,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -4085,6 +4073,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -4837,69 +4837,69 @@
       <c r="BA5" s="47"/>
       <c r="BB5" s="47"/>
     </row>
-    <row r="6" spans="1:54" s="126" customFormat="1">
-      <c r="A6" s="119"/>
-      <c r="B6" s="120" t="s">
+    <row r="6" spans="1:54" s="122" customFormat="1">
+      <c r="A6" s="115"/>
+      <c r="B6" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="119">
+      <c r="C6" s="115">
         <v>1</v>
       </c>
-      <c r="D6" s="119">
+      <c r="D6" s="115">
         <v>1</v>
       </c>
-      <c r="E6" s="121"/>
-      <c r="F6" s="122"/>
-      <c r="G6" s="122"/>
-      <c r="H6" s="123"/>
-      <c r="I6" s="123"/>
-      <c r="J6" s="124">
+      <c r="E6" s="117"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="119"/>
+      <c r="J6" s="120">
         <v>1</v>
       </c>
-      <c r="K6" s="123"/>
-      <c r="L6" s="123"/>
-      <c r="M6" s="123"/>
-      <c r="N6" s="125"/>
-      <c r="O6" s="123"/>
-      <c r="P6" s="123"/>
-      <c r="Q6" s="123"/>
-      <c r="R6" s="123"/>
-      <c r="S6" s="123"/>
-      <c r="T6" s="124"/>
-      <c r="U6" s="123"/>
-      <c r="V6" s="123"/>
-      <c r="W6" s="123"/>
-      <c r="X6" s="125"/>
-      <c r="Y6" s="124"/>
-      <c r="Z6" s="123"/>
-      <c r="AA6" s="123"/>
-      <c r="AB6" s="123"/>
-      <c r="AC6" s="125"/>
-      <c r="AD6" s="124"/>
-      <c r="AE6" s="123"/>
-      <c r="AF6" s="123"/>
-      <c r="AG6" s="123"/>
-      <c r="AH6" s="125"/>
-      <c r="AI6" s="123"/>
-      <c r="AJ6" s="124"/>
-      <c r="AK6" s="123"/>
-      <c r="AL6" s="123"/>
-      <c r="AM6" s="123"/>
-      <c r="AN6" s="125"/>
-      <c r="AO6" s="124"/>
-      <c r="AP6" s="123"/>
-      <c r="AQ6" s="123"/>
-      <c r="AR6" s="123"/>
-      <c r="AS6" s="125"/>
-      <c r="AT6" s="124"/>
-      <c r="AU6" s="123"/>
-      <c r="AV6" s="123"/>
-      <c r="AW6" s="123"/>
-      <c r="AX6" s="125"/>
-      <c r="AY6" s="119"/>
-      <c r="AZ6" s="119"/>
-      <c r="BA6" s="119"/>
-      <c r="BB6" s="119"/>
+      <c r="K6" s="119"/>
+      <c r="L6" s="119"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="121"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="119"/>
+      <c r="Q6" s="119"/>
+      <c r="R6" s="119"/>
+      <c r="S6" s="119"/>
+      <c r="T6" s="120"/>
+      <c r="U6" s="119"/>
+      <c r="V6" s="119"/>
+      <c r="W6" s="119"/>
+      <c r="X6" s="121"/>
+      <c r="Y6" s="120"/>
+      <c r="Z6" s="119"/>
+      <c r="AA6" s="119"/>
+      <c r="AB6" s="119"/>
+      <c r="AC6" s="121"/>
+      <c r="AD6" s="120"/>
+      <c r="AE6" s="119"/>
+      <c r="AF6" s="119"/>
+      <c r="AG6" s="119"/>
+      <c r="AH6" s="121"/>
+      <c r="AI6" s="119"/>
+      <c r="AJ6" s="120"/>
+      <c r="AK6" s="119"/>
+      <c r="AL6" s="119"/>
+      <c r="AM6" s="119"/>
+      <c r="AN6" s="121"/>
+      <c r="AO6" s="120"/>
+      <c r="AP6" s="119"/>
+      <c r="AQ6" s="119"/>
+      <c r="AR6" s="119"/>
+      <c r="AS6" s="121"/>
+      <c r="AT6" s="120"/>
+      <c r="AU6" s="119"/>
+      <c r="AV6" s="119"/>
+      <c r="AW6" s="119"/>
+      <c r="AX6" s="121"/>
+      <c r="AY6" s="115"/>
+      <c r="AZ6" s="115"/>
+      <c r="BA6" s="115"/>
+      <c r="BB6" s="115"/>
     </row>
     <row r="7" spans="1:54">
       <c r="A7" s="47"/>
@@ -5047,67 +5047,67 @@
       <c r="BA8" s="47"/>
       <c r="BB8" s="47"/>
     </row>
-    <row r="9" spans="1:54" s="126" customFormat="1">
-      <c r="B9" s="119" t="s">
+    <row r="9" spans="1:54" s="122" customFormat="1">
+      <c r="B9" s="115" t="s">
         <v>288</v>
       </c>
-      <c r="C9" s="119">
+      <c r="C9" s="115">
         <v>1</v>
       </c>
-      <c r="D9" s="119">
+      <c r="D9" s="115">
         <v>1</v>
       </c>
-      <c r="E9" s="121"/>
-      <c r="F9" s="122"/>
-      <c r="G9" s="122"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="124"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
-      <c r="M9" s="123"/>
-      <c r="N9" s="125"/>
-      <c r="O9" s="123"/>
-      <c r="P9" s="123"/>
-      <c r="Q9" s="123"/>
-      <c r="R9" s="123"/>
-      <c r="S9" s="123"/>
-      <c r="T9" s="124"/>
-      <c r="U9" s="123">
+      <c r="E9" s="117"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
+      <c r="H9" s="119"/>
+      <c r="I9" s="119"/>
+      <c r="J9" s="120"/>
+      <c r="K9" s="119"/>
+      <c r="L9" s="119"/>
+      <c r="M9" s="119"/>
+      <c r="N9" s="121"/>
+      <c r="O9" s="119"/>
+      <c r="P9" s="119"/>
+      <c r="Q9" s="119"/>
+      <c r="R9" s="119"/>
+      <c r="S9" s="119"/>
+      <c r="T9" s="120"/>
+      <c r="U9" s="119">
         <v>1</v>
       </c>
-      <c r="W9" s="123"/>
-      <c r="X9" s="125"/>
-      <c r="Y9" s="124"/>
-      <c r="Z9" s="123"/>
-      <c r="AA9" s="123"/>
-      <c r="AB9" s="123"/>
-      <c r="AC9" s="125"/>
-      <c r="AD9" s="124"/>
-      <c r="AE9" s="123"/>
-      <c r="AF9" s="123"/>
-      <c r="AG9" s="123"/>
-      <c r="AH9" s="125"/>
-      <c r="AI9" s="123"/>
-      <c r="AJ9" s="124"/>
-      <c r="AK9" s="123"/>
-      <c r="AL9" s="123"/>
-      <c r="AM9" s="123"/>
-      <c r="AN9" s="125"/>
-      <c r="AO9" s="124"/>
-      <c r="AP9" s="123"/>
-      <c r="AQ9" s="123"/>
-      <c r="AR9" s="123"/>
-      <c r="AS9" s="125"/>
-      <c r="AT9" s="124"/>
-      <c r="AU9" s="123"/>
-      <c r="AV9" s="123"/>
-      <c r="AW9" s="123"/>
-      <c r="AX9" s="125"/>
-      <c r="AY9" s="119"/>
-      <c r="AZ9" s="119"/>
-      <c r="BA9" s="119"/>
-      <c r="BB9" s="119"/>
+      <c r="W9" s="119"/>
+      <c r="X9" s="121"/>
+      <c r="Y9" s="120"/>
+      <c r="Z9" s="119"/>
+      <c r="AA9" s="119"/>
+      <c r="AB9" s="119"/>
+      <c r="AC9" s="121"/>
+      <c r="AD9" s="120"/>
+      <c r="AE9" s="119"/>
+      <c r="AF9" s="119"/>
+      <c r="AG9" s="119"/>
+      <c r="AH9" s="121"/>
+      <c r="AI9" s="119"/>
+      <c r="AJ9" s="120"/>
+      <c r="AK9" s="119"/>
+      <c r="AL9" s="119"/>
+      <c r="AM9" s="119"/>
+      <c r="AN9" s="121"/>
+      <c r="AO9" s="120"/>
+      <c r="AP9" s="119"/>
+      <c r="AQ9" s="119"/>
+      <c r="AR9" s="119"/>
+      <c r="AS9" s="121"/>
+      <c r="AT9" s="120"/>
+      <c r="AU9" s="119"/>
+      <c r="AV9" s="119"/>
+      <c r="AW9" s="119"/>
+      <c r="AX9" s="121"/>
+      <c r="AY9" s="115"/>
+      <c r="AZ9" s="115"/>
+      <c r="BA9" s="115"/>
+      <c r="BB9" s="115"/>
     </row>
     <row r="10" spans="1:54">
       <c r="A10" s="47"/>
@@ -5285,71 +5285,71 @@
       <c r="BA11" s="47"/>
       <c r="BB11" s="47"/>
     </row>
-    <row r="12" spans="1:54" s="126" customFormat="1">
-      <c r="A12" s="119"/>
-      <c r="B12" s="119" t="s">
+    <row r="12" spans="1:54" s="122" customFormat="1">
+      <c r="A12" s="115"/>
+      <c r="B12" s="115" t="s">
         <v>429</v>
       </c>
-      <c r="C12" s="119">
+      <c r="C12" s="115">
         <v>2</v>
       </c>
-      <c r="D12" s="119">
+      <c r="D12" s="115">
         <v>2</v>
       </c>
-      <c r="E12" s="121"/>
-      <c r="F12" s="122"/>
-      <c r="G12" s="122"/>
-      <c r="H12" s="123"/>
-      <c r="I12" s="123"/>
-      <c r="J12" s="124"/>
-      <c r="K12" s="123"/>
-      <c r="L12" s="123"/>
-      <c r="M12" s="123"/>
-      <c r="N12" s="125"/>
-      <c r="O12" s="123"/>
-      <c r="P12" s="123"/>
-      <c r="Q12" s="123"/>
-      <c r="R12" s="123"/>
-      <c r="S12" s="123"/>
-      <c r="T12" s="124"/>
-      <c r="U12" s="123"/>
-      <c r="V12" s="123"/>
-      <c r="W12" s="123"/>
-      <c r="X12" s="125"/>
-      <c r="Y12" s="124"/>
-      <c r="Z12" s="123"/>
-      <c r="AA12" s="123"/>
-      <c r="AB12" s="123"/>
-      <c r="AC12" s="125"/>
-      <c r="AD12" s="124"/>
-      <c r="AE12" s="123"/>
-      <c r="AF12" s="123"/>
-      <c r="AG12" s="123"/>
-      <c r="AH12" s="125"/>
-      <c r="AI12" s="123"/>
-      <c r="AJ12" s="124"/>
-      <c r="AK12" s="123"/>
-      <c r="AL12" s="123"/>
-      <c r="AM12" s="123"/>
-      <c r="AN12" s="125"/>
-      <c r="AO12" s="124"/>
-      <c r="AP12" s="123">
+      <c r="E12" s="117"/>
+      <c r="F12" s="118"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="119"/>
+      <c r="I12" s="119"/>
+      <c r="J12" s="120"/>
+      <c r="K12" s="119"/>
+      <c r="L12" s="119"/>
+      <c r="M12" s="119"/>
+      <c r="N12" s="121"/>
+      <c r="O12" s="119"/>
+      <c r="P12" s="119"/>
+      <c r="Q12" s="119"/>
+      <c r="R12" s="119"/>
+      <c r="S12" s="119"/>
+      <c r="T12" s="120"/>
+      <c r="U12" s="119"/>
+      <c r="V12" s="119"/>
+      <c r="W12" s="119"/>
+      <c r="X12" s="121"/>
+      <c r="Y12" s="120"/>
+      <c r="Z12" s="119"/>
+      <c r="AA12" s="119"/>
+      <c r="AB12" s="119"/>
+      <c r="AC12" s="121"/>
+      <c r="AD12" s="120"/>
+      <c r="AE12" s="119"/>
+      <c r="AF12" s="119"/>
+      <c r="AG12" s="119"/>
+      <c r="AH12" s="121"/>
+      <c r="AI12" s="119"/>
+      <c r="AJ12" s="120"/>
+      <c r="AK12" s="119"/>
+      <c r="AL12" s="119"/>
+      <c r="AM12" s="119"/>
+      <c r="AN12" s="121"/>
+      <c r="AO12" s="120"/>
+      <c r="AP12" s="119">
         <v>1</v>
       </c>
-      <c r="AQ12" s="123">
+      <c r="AQ12" s="119">
         <v>1</v>
       </c>
-      <c r="AR12" s="123"/>
-      <c r="AS12" s="125"/>
-      <c r="AT12" s="124"/>
-      <c r="AU12" s="123"/>
-      <c r="AV12" s="123"/>
-      <c r="AW12" s="123"/>
-      <c r="AX12" s="125"/>
-      <c r="AY12" s="119"/>
-      <c r="AZ12" s="119"/>
-      <c r="BA12" s="119"/>
-      <c r="BB12" s="119"/>
+      <c r="AR12" s="119"/>
+      <c r="AS12" s="121"/>
+      <c r="AT12" s="120"/>
+      <c r="AU12" s="119"/>
+      <c r="AV12" s="119"/>
+      <c r="AW12" s="119"/>
+      <c r="AX12" s="121"/>
+      <c r="AY12" s="115"/>
+      <c r="AZ12" s="115"/>
+      <c r="BA12" s="115"/>
+      <c r="BB12" s="115"/>
     </row>
     <row r="13" spans="1:54">
       <c r="A13" s="47" t="s">
@@ -61361,7 +61361,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B19" sqref="B2:B19"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.9140625" defaultRowHeight="14.5"/>
@@ -61450,37 +61450,37 @@
       <c r="K2" s="16"/>
       <c r="L2" s="17"/>
     </row>
-    <row r="3" spans="1:12" s="111" customFormat="1" ht="29">
-      <c r="A3" s="111">
+    <row r="3" spans="1:12" s="107" customFormat="1" ht="29">
+      <c r="A3" s="107">
         <v>1</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="108" t="s">
         <v>318</v>
       </c>
-      <c r="C3" s="113" t="s">
+      <c r="C3" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="109" t="s">
         <v>319</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="109" t="s">
         <v>444</v>
       </c>
-      <c r="F3" s="113"/>
-      <c r="G3" s="113"/>
-      <c r="H3" s="113" t="s">
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109" t="s">
         <v>390</v>
       </c>
-      <c r="I3" s="114" t="s">
+      <c r="I3" s="110" t="s">
         <v>321</v>
       </c>
-      <c r="J3" s="113" t="s">
+      <c r="J3" s="109" t="s">
         <v>320</v>
       </c>
-      <c r="K3" s="114" t="s">
+      <c r="K3" s="110" t="s">
         <v>133</v>
       </c>
-      <c r="L3" s="115"/>
+      <c r="L3" s="111"/>
     </row>
     <row r="4" spans="1:12" s="30" customFormat="1" ht="29">
       <c r="A4" s="18">
@@ -61780,33 +61780,33 @@
       <c r="K13" s="33"/>
       <c r="L13" s="35"/>
     </row>
-    <row r="14" spans="1:12" s="84" customFormat="1">
-      <c r="A14" s="84">
+    <row r="14" spans="1:12" s="123" customFormat="1">
+      <c r="A14" s="123">
         <v>11</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="124" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="86" t="s">
+      <c r="C14" s="125" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="86" t="s">
+      <c r="D14" s="125" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="87" t="s">
+      <c r="E14" s="125"/>
+      <c r="F14" s="125"/>
+      <c r="G14" s="125"/>
+      <c r="H14" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="I14" s="87"/>
-      <c r="J14" s="87" t="s">
+      <c r="I14" s="83"/>
+      <c r="J14" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="K14" s="87" t="s">
+      <c r="K14" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="L14" s="88" t="s">
+      <c r="L14" s="126" t="s">
         <v>212</v>
       </c>
     </row>
@@ -61868,33 +61868,33 @@
       <c r="K16" s="33"/>
       <c r="L16" s="35"/>
     </row>
-    <row r="17" spans="1:12" s="89" customFormat="1" ht="29">
-      <c r="A17" s="89">
+    <row r="17" spans="1:12" s="85" customFormat="1" ht="29">
+      <c r="A17" s="85">
         <v>14</v>
       </c>
-      <c r="B17" s="90" t="s">
+      <c r="B17" s="86" t="s">
         <v>129</v>
       </c>
-      <c r="C17" s="91" t="s">
+      <c r="C17" s="87" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="91" t="s">
+      <c r="D17" s="87" t="s">
         <v>130</v>
       </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="91"/>
-      <c r="G17" s="91"/>
-      <c r="H17" s="92" t="s">
+      <c r="E17" s="88"/>
+      <c r="F17" s="87"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="88" t="s">
         <v>132</v>
       </c>
-      <c r="I17" s="92" t="s">
+      <c r="I17" s="88" t="s">
         <v>138</v>
       </c>
-      <c r="J17" s="91" t="s">
+      <c r="J17" s="87" t="s">
         <v>131</v>
       </c>
-      <c r="K17" s="91"/>
-      <c r="L17" s="88" t="s">
+      <c r="K17" s="87"/>
+      <c r="L17" s="84" t="s">
         <v>212</v>
       </c>
     </row>
@@ -62087,8 +62087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6EF2C2-8F5D-482B-8D1B-02457D7267B7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -62109,10 +62109,10 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="101.5">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="89" t="s">
         <v>181</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="89" t="s">
         <v>182</v>
       </c>
     </row>
@@ -62213,53 +62213,53 @@
       </c>
       <c r="M1" s="65"/>
     </row>
-    <row r="2" spans="1:13" s="99" customFormat="1" ht="43.5">
-      <c r="A2" s="96" t="s">
+    <row r="2" spans="1:13" s="95" customFormat="1" ht="43.5">
+      <c r="A2" s="92" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="102" t="s">
+      <c r="B2" s="92"/>
+      <c r="C2" s="98" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="97"/>
-      <c r="E2" s="97"/>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97" t="s">
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93" t="s">
         <v>302</v>
       </c>
-      <c r="H2" s="97" t="s">
+      <c r="H2" s="93" t="s">
         <v>251</v>
       </c>
-      <c r="I2" s="97" t="s">
+      <c r="I2" s="93" t="s">
         <v>254</v>
       </c>
-      <c r="J2" s="97"/>
-      <c r="K2" s="97"/>
-      <c r="L2" s="97" t="s">
+      <c r="J2" s="93"/>
+      <c r="K2" s="93"/>
+      <c r="L2" s="93" t="s">
         <v>246</v>
       </c>
-      <c r="M2" s="98"/>
-    </row>
-    <row r="3" spans="1:13" s="99" customFormat="1" ht="29">
-      <c r="A3" s="96"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="102" t="s">
+      <c r="M2" s="94"/>
+    </row>
+    <row r="3" spans="1:13" s="95" customFormat="1" ht="29">
+      <c r="A3" s="92"/>
+      <c r="B3" s="92"/>
+      <c r="C3" s="98" t="s">
         <v>258</v>
       </c>
-      <c r="D3" s="97"/>
-      <c r="E3" s="97"/>
-      <c r="F3" s="97"/>
-      <c r="G3" s="97" t="s">
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93" t="s">
         <v>259</v>
       </c>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="93" t="s">
         <v>251</v>
       </c>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
-      <c r="K3" s="97"/>
-      <c r="L3" s="97"/>
-      <c r="M3" s="98"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
+      <c r="M3" s="94"/>
     </row>
     <row r="4" spans="1:13" ht="72.5">
       <c r="A4" s="67" t="s">
@@ -62268,7 +62268,7 @@
       <c r="B4" s="67" t="s">
         <v>261</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="97" t="s">
         <v>262</v>
       </c>
       <c r="D4" s="68" t="s">
@@ -62299,7 +62299,7 @@
       <c r="B5" s="67" t="s">
         <v>193</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="97" t="s">
         <v>160</v>
       </c>
       <c r="D5" s="68" t="s">
@@ -62326,7 +62326,7 @@
       <c r="B6" s="67" t="s">
         <v>191</v>
       </c>
-      <c r="C6" s="101" t="s">
+      <c r="C6" s="97" t="s">
         <v>159</v>
       </c>
       <c r="D6" s="68" t="s">
@@ -62351,7 +62351,7 @@
       <c r="B7" s="67" t="s">
         <v>192</v>
       </c>
-      <c r="C7" s="101" t="s">
+      <c r="C7" s="97" t="s">
         <v>284</v>
       </c>
       <c r="D7" s="68" t="s">
@@ -62376,7 +62376,7 @@
       <c r="B8" s="77" t="s">
         <v>292</v>
       </c>
-      <c r="C8" s="100" t="s">
+      <c r="C8" s="96" t="s">
         <v>296</v>
       </c>
       <c r="D8" s="77" t="s">
@@ -62408,7 +62408,7 @@
         <v>205</v>
       </c>
       <c r="B9" s="76"/>
-      <c r="C9" s="100" t="s">
+      <c r="C9" s="96" t="s">
         <v>278</v>
       </c>
       <c r="D9" s="77"/>
@@ -62434,7 +62434,7 @@
         <v>206</v>
       </c>
       <c r="B10" s="76"/>
-      <c r="C10" s="100" t="s">
+      <c r="C10" s="96" t="s">
         <v>198</v>
       </c>
       <c r="D10" s="76"/>
@@ -62460,7 +62460,7 @@
       <c r="B11" s="72" t="s">
         <v>194</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="99" t="s">
         <v>161</v>
       </c>
       <c r="D11" s="73" t="s">
@@ -62497,7 +62497,7 @@
       <c r="B12" s="72" t="s">
         <v>353</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="99" t="s">
         <v>352</v>
       </c>
       <c r="D12" s="73"/>
@@ -62512,7 +62512,7 @@
         <v>380</v>
       </c>
       <c r="I12" s="73"/>
-      <c r="J12" s="109" t="s">
+      <c r="J12" s="105" t="s">
         <v>378</v>
       </c>
       <c r="K12" s="73" t="s">
@@ -62528,7 +62528,7 @@
       <c r="B13" s="72" t="s">
         <v>217</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="99" t="s">
         <v>218</v>
       </c>
       <c r="D13" s="73" t="s">
@@ -62563,7 +62563,7 @@
       <c r="B14" s="72" t="s">
         <v>195</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="99" t="s">
         <v>164</v>
       </c>
       <c r="D14" s="73" t="s">
@@ -62594,7 +62594,7 @@
       <c r="B15" s="79" t="s">
         <v>196</v>
       </c>
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="100" t="s">
         <v>163</v>
       </c>
       <c r="D15" s="80" t="s">
@@ -62627,7 +62627,7 @@
       <c r="B16" s="79" t="s">
         <v>197</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="100" t="s">
         <v>162</v>
       </c>
       <c r="D16" s="80" t="s">
@@ -62642,7 +62642,7 @@
       </c>
       <c r="H16" s="80"/>
       <c r="I16" s="80"/>
-      <c r="J16" s="106" t="s">
+      <c r="J16" s="102" t="s">
         <v>362</v>
       </c>
       <c r="K16" s="80"/>
@@ -62654,7 +62654,7 @@
         <v>96</v>
       </c>
       <c r="B17" s="67"/>
-      <c r="C17" s="101" t="s">
+      <c r="C17" s="97" t="s">
         <v>153</v>
       </c>
       <c r="D17" s="68" t="s">
@@ -62676,7 +62676,7 @@
     <row r="18" spans="1:12" s="71" customFormat="1" ht="145">
       <c r="A18" s="67"/>
       <c r="B18" s="67"/>
-      <c r="C18" s="101" t="s">
+      <c r="C18" s="97" t="s">
         <v>279</v>
       </c>
       <c r="D18" s="68" t="s">
@@ -62698,7 +62698,7 @@
     <row r="19" spans="1:12" s="71" customFormat="1" ht="29">
       <c r="A19" s="67"/>
       <c r="B19" s="67"/>
-      <c r="C19" s="101" t="s">
+      <c r="C19" s="97" t="s">
         <v>399</v>
       </c>
       <c r="D19" s="68" t="s">
@@ -62711,7 +62711,7 @@
         <v>337</v>
       </c>
       <c r="I19" s="68"/>
-      <c r="J19" s="107" t="s">
+      <c r="J19" s="103" t="s">
         <v>338</v>
       </c>
       <c r="K19" s="67"/>
@@ -62720,7 +62720,7 @@
     <row r="20" spans="1:12" s="71" customFormat="1" ht="29">
       <c r="A20" s="67"/>
       <c r="B20" s="67"/>
-      <c r="C20" s="101" t="s">
+      <c r="C20" s="97" t="s">
         <v>400</v>
       </c>
       <c r="D20" s="68" t="s">
@@ -62733,7 +62733,7 @@
         <v>401</v>
       </c>
       <c r="I20" s="68"/>
-      <c r="J20" s="107"/>
+      <c r="J20" s="103"/>
       <c r="K20" s="67"/>
       <c r="L20" s="68"/>
     </row>
@@ -62757,7 +62757,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="24.5" customHeight="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="112" t="s">
         <v>434</v>
       </c>
     </row>
@@ -63028,262 +63028,262 @@
       </c>
       <c r="I13" s="26"/>
     </row>
-    <row r="14" spans="1:9" s="108" customFormat="1" ht="43.5">
-      <c r="A14" s="94" t="s">
+    <row r="14" spans="1:9" s="104" customFormat="1" ht="43.5">
+      <c r="A14" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="90" t="s">
         <v>233</v>
       </c>
-      <c r="C14" s="94" t="s">
+      <c r="C14" s="90" t="s">
         <v>435</v>
       </c>
-      <c r="D14" s="94" t="s">
+      <c r="D14" s="90" t="s">
         <v>326</v>
       </c>
-      <c r="E14" s="95" t="s">
+      <c r="E14" s="91" t="s">
         <v>305</v>
       </c>
-      <c r="F14" s="95" t="s">
+      <c r="F14" s="91" t="s">
         <v>289</v>
       </c>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
-      <c r="I14" s="95"/>
+      <c r="G14" s="91"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="91"/>
     </row>
     <row r="15" spans="1:9" ht="43.5">
-      <c r="A15" s="94" t="s">
+      <c r="A15" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="94" t="s">
+      <c r="B15" s="90" t="s">
         <v>371</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="91" t="s">
         <v>372</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="91" t="s">
         <v>374</v>
       </c>
-      <c r="E15" s="95" t="s">
+      <c r="E15" s="91" t="s">
         <v>375</v>
       </c>
-      <c r="F15" s="95" t="s">
+      <c r="F15" s="91" t="s">
         <v>373</v>
       </c>
-      <c r="G15" s="95" t="s">
+      <c r="G15" s="91" t="s">
         <v>376</v>
       </c>
-      <c r="H15" s="95"/>
-      <c r="I15" s="95"/>
-    </row>
-    <row r="16" spans="1:9" s="108" customFormat="1" ht="43.5">
-      <c r="A16" s="94" t="s">
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+    </row>
+    <row r="16" spans="1:9" s="104" customFormat="1" ht="43.5">
+      <c r="A16" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="B16" s="94" t="s">
+      <c r="B16" s="90" t="s">
         <v>213</v>
       </c>
-      <c r="C16" s="95" t="s">
+      <c r="C16" s="91" t="s">
         <v>360</v>
       </c>
-      <c r="D16" s="95"/>
-      <c r="E16" s="95" t="s">
+      <c r="D16" s="91"/>
+      <c r="E16" s="91" t="s">
         <v>309</v>
       </c>
-      <c r="F16" s="95" t="s">
+      <c r="F16" s="91" t="s">
         <v>351</v>
       </c>
-      <c r="G16" s="95" t="s">
+      <c r="G16" s="91" t="s">
         <v>270</v>
       </c>
-      <c r="H16" s="95" t="s">
+      <c r="H16" s="91" t="s">
         <v>238</v>
       </c>
-      <c r="I16" s="95" t="s">
+      <c r="I16" s="91" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="108" customFormat="1" ht="43.5">
-      <c r="A17" s="94" t="s">
+    <row r="17" spans="1:9" s="104" customFormat="1" ht="43.5">
+      <c r="A17" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="90" t="s">
         <v>215</v>
       </c>
-      <c r="C17" s="95" t="s">
+      <c r="C17" s="91" t="s">
         <v>377</v>
       </c>
-      <c r="D17" s="95"/>
-      <c r="E17" s="95" t="s">
+      <c r="D17" s="91"/>
+      <c r="E17" s="91" t="s">
         <v>310</v>
       </c>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95" t="s">
+      <c r="F17" s="91"/>
+      <c r="G17" s="91" t="s">
         <v>271</v>
       </c>
-      <c r="H17" s="94" t="s">
+      <c r="H17" s="90" t="s">
         <v>194</v>
       </c>
-      <c r="I17" s="95" t="s">
+      <c r="I17" s="91" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="108" customFormat="1" ht="43.5">
-      <c r="A18" s="94" t="s">
+    <row r="18" spans="1:9" s="104" customFormat="1" ht="43.5">
+      <c r="A18" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="B18" s="94" t="s">
+      <c r="B18" s="90" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="94" t="s">
+      <c r="C18" s="90" t="s">
         <v>227</v>
       </c>
-      <c r="D18" s="94"/>
-      <c r="E18" s="95" t="s">
+      <c r="D18" s="90"/>
+      <c r="E18" s="91" t="s">
         <v>240</v>
       </c>
-      <c r="F18" s="95"/>
-      <c r="G18" s="95" t="s">
+      <c r="F18" s="91"/>
+      <c r="G18" s="91" t="s">
         <v>273</v>
       </c>
-      <c r="H18" s="95" t="s">
+      <c r="H18" s="91" t="s">
         <v>239</v>
       </c>
-      <c r="I18" s="95" t="s">
+      <c r="I18" s="91" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="29">
-      <c r="A19" s="94" t="s">
+      <c r="A19" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="90" t="s">
         <v>361</v>
       </c>
-      <c r="C19" s="95" t="s">
+      <c r="C19" s="91" t="s">
         <v>348</v>
       </c>
-      <c r="D19" s="95" t="s">
+      <c r="D19" s="91" t="s">
         <v>327</v>
       </c>
-      <c r="E19" s="95" t="s">
+      <c r="E19" s="91" t="s">
         <v>236</v>
       </c>
-      <c r="F19" s="95" t="s">
+      <c r="F19" s="91" t="s">
         <v>324</v>
       </c>
-      <c r="G19" s="95" t="s">
+      <c r="G19" s="91" t="s">
         <v>274</v>
       </c>
-      <c r="H19" s="95"/>
-      <c r="I19" s="95" t="s">
+      <c r="H19" s="91"/>
+      <c r="I19" s="91" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="14.5">
-      <c r="A20" s="94" t="s">
+      <c r="A20" s="90" t="s">
         <v>425</v>
       </c>
-      <c r="B20" s="94" t="s">
+      <c r="B20" s="90" t="s">
         <v>426</v>
       </c>
-      <c r="C20" s="95"/>
-      <c r="D20" s="95"/>
-      <c r="E20" s="95"/>
-      <c r="F20" s="95" t="s">
+      <c r="C20" s="91"/>
+      <c r="D20" s="91"/>
+      <c r="E20" s="91"/>
+      <c r="F20" s="91" t="s">
         <v>427</v>
       </c>
-      <c r="G20" s="95"/>
-      <c r="H20" s="95"/>
-      <c r="I20" s="95"/>
+      <c r="G20" s="91"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
     </row>
     <row r="21" spans="1:9" s="31" customFormat="1" ht="30" customHeight="1">
-      <c r="A21" s="94" t="s">
+      <c r="A21" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="90" t="s">
         <v>363</v>
       </c>
-      <c r="C21" s="94" t="s">
+      <c r="C21" s="90" t="s">
         <v>347</v>
       </c>
-      <c r="D21" s="94" t="s">
+      <c r="D21" s="90" t="s">
         <v>326</v>
       </c>
-      <c r="E21" s="95" t="s">
+      <c r="E21" s="91" t="s">
         <v>334</v>
       </c>
-      <c r="F21" s="95" t="s">
+      <c r="F21" s="91" t="s">
         <v>323</v>
       </c>
-      <c r="G21" s="95"/>
-      <c r="H21" s="95"/>
-      <c r="I21" s="95"/>
+      <c r="G21" s="91"/>
+      <c r="H21" s="91"/>
+      <c r="I21" s="91"/>
     </row>
     <row r="22" spans="1:9" ht="14.5">
-      <c r="A22" s="94" t="s">
+      <c r="A22" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="94" t="s">
+      <c r="B22" s="90" t="s">
         <v>328</v>
       </c>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95" t="s">
+      <c r="C22" s="91"/>
+      <c r="D22" s="91" t="s">
         <v>327</v>
       </c>
-      <c r="E22" s="95" t="s">
+      <c r="E22" s="91" t="s">
         <v>335</v>
       </c>
-      <c r="F22" s="95" t="s">
+      <c r="F22" s="91" t="s">
         <v>329</v>
       </c>
-      <c r="G22" s="95"/>
-      <c r="H22" s="95"/>
-      <c r="I22" s="95"/>
+      <c r="G22" s="91"/>
+      <c r="H22" s="91"/>
+      <c r="I22" s="91"/>
     </row>
     <row r="23" spans="1:9" ht="14.5">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="94" t="s">
+      <c r="B23" s="90" t="s">
         <v>330</v>
       </c>
-      <c r="C23" s="95"/>
-      <c r="D23" s="95"/>
-      <c r="E23" s="95" t="s">
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91" t="s">
         <v>335</v>
       </c>
-      <c r="F23" s="95" t="s">
+      <c r="F23" s="91" t="s">
         <v>332</v>
       </c>
-      <c r="G23" s="95"/>
-      <c r="H23" s="95"/>
-      <c r="I23" s="95"/>
+      <c r="G23" s="91"/>
+      <c r="H23" s="91"/>
+      <c r="I23" s="91"/>
     </row>
     <row r="24" spans="1:9" ht="14.5">
-      <c r="A24" s="94" t="s">
+      <c r="A24" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="94" t="s">
+      <c r="B24" s="90" t="s">
         <v>331</v>
       </c>
-      <c r="C24" s="95"/>
-      <c r="D24" s="95"/>
-      <c r="E24" s="95" t="s">
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="91" t="s">
         <v>335</v>
       </c>
-      <c r="F24" s="95" t="s">
+      <c r="F24" s="91" t="s">
         <v>333</v>
       </c>
-      <c r="G24" s="95"/>
-      <c r="H24" s="95"/>
-      <c r="I24" s="95"/>
-    </row>
-    <row r="25" spans="1:9" s="118" customFormat="1" ht="43.5">
+      <c r="G24" s="91"/>
+      <c r="H24" s="91"/>
+      <c r="I24" s="91"/>
+    </row>
+    <row r="25" spans="1:9" s="114" customFormat="1" ht="43.5">
       <c r="A25" s="79" t="s">
         <v>442</v>
       </c>
-      <c r="B25" s="117" t="s">
+      <c r="B25" s="113" t="s">
         <v>441</v>
       </c>
       <c r="C25" s="80" t="s">
@@ -63300,7 +63300,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="118" customFormat="1" ht="14.5">
+    <row r="26" spans="1:9" s="114" customFormat="1" ht="14.5">
       <c r="A26" s="79" t="s">
         <v>442</v>
       </c>
@@ -63315,7 +63315,7 @@
       <c r="H26" s="80"/>
       <c r="I26" s="80"/>
     </row>
-    <row r="27" spans="1:9" s="118" customFormat="1" ht="14.5">
+    <row r="27" spans="1:9" s="114" customFormat="1" ht="14.5">
       <c r="A27" s="79" t="s">
         <v>442</v>
       </c>
@@ -63421,21 +63421,21 @@
       <c r="I31" s="24"/>
     </row>
     <row r="32" spans="1:9" s="31" customFormat="1" ht="30" customHeight="1">
-      <c r="A32" s="105" t="s">
+      <c r="A32" s="101" t="s">
         <v>267</v>
       </c>
-      <c r="B32" s="105" t="s">
+      <c r="B32" s="101" t="s">
         <v>343</v>
       </c>
-      <c r="C32" s="105" t="s">
+      <c r="C32" s="101" t="s">
         <v>344</v>
       </c>
-      <c r="D32" s="105"/>
-      <c r="E32" s="105"/>
-      <c r="F32" s="105"/>
-      <c r="G32" s="105"/>
-      <c r="H32" s="105"/>
-      <c r="I32" s="105"/>
+      <c r="D32" s="101"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="101"/>
+      <c r="G32" s="101"/>
+      <c r="H32" s="101"/>
+      <c r="I32" s="101"/>
     </row>
     <row r="33" spans="1:9" ht="30" customHeight="1">
       <c r="A33" s="24" t="s">
@@ -63537,7 +63537,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="106" t="s">
         <v>385</v>
       </c>
       <c r="B4" t="s">

</xml_diff>